<commit_message>
Few comments were added
</commit_message>
<xml_diff>
--- a/highbond_api_call_list.xlsx
+++ b/highbond_api_call_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NandhiniRamachandran\Documents\Windstream\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BD0ADF-2387-4B3C-AFD7-3303228E6ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F748B244-AC09-4E41-9D8D-D2252FDE300C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{980EFD35-49B2-4B62-A449-1140250EE396}"/>
   </bookViews>
@@ -837,7 +837,7 @@
   <dimension ref="A2:D136"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Access credential input file (#3)
* Added tables in excel sheet

* added few comments and removed the function export to excel with list of df as an argument

* Deleted the function which is not required and added few more comments in the code

* " added dynamic input for region code"

* Few comments were added

* created an input file to read multiple org id
</commit_message>
<xml_diff>
--- a/highbond_api_call_list.xlsx
+++ b/highbond_api_call_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NandhiniRamachandran\Documents\Windstream\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BD0ADF-2387-4B3C-AFD7-3303228E6ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F748B244-AC09-4E41-9D8D-D2252FDE300C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{980EFD35-49B2-4B62-A449-1140250EE396}"/>
   </bookViews>
@@ -837,7 +837,7 @@
   <dimension ref="A2:D136"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>